<commit_message>
Finished important resources and examples
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-ncdth-allergy-intolerance.xlsx
+++ b/output/StructureDefinition-ncdth-allergy-intolerance.xlsx
@@ -9,11 +9,14 @@
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AL$36</definedName>
+  </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="321">
   <si>
     <t>Property</t>
   </si>
@@ -42,7 +45,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>NCD Thailand AllergyIntolerance Profile</t>
+    <t>NCD TH AllergyIntolerance Profile</t>
   </si>
   <si>
     <t>Status</t>
@@ -57,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-02-22T11:05:10+07:00</t>
+    <t>2022-02-22T23:30:09+07:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -648,10 +651,7 @@
 The 'substanceExposureRisk' extension is available as a structured and more flexible alternative to the 'code' element for making positive or negative allergy or intolerance statements.  This extension provides the capability to make "no known allergy" (or "no risk of adverse reaction") statements regarding any coded substance/product (including cases when a pre-coordinated "no allergy to x" concept for that substance/product does not exist).  If the 'substanceExposureRisk' extension is present, the AllergyIntolerance.code element SHALL be omitted.</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>Type of the substance/product, allergy or intolerance condition, or negation/exclusion codes for reporting no known allergies.</t>
+    <t>extensible</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/allergyintolerance-code</t>
@@ -917,6 +917,9 @@
     <t>Coding of the specific substance (or pharmaceutical product) with a terminology capable of triggering decision support should be used wherever possible.  The 'code' element allows for the use of a specific substance or pharmaceutical product, or a group or class of substances. In the case of an allergy or intolerance to a class of substances, (for example, "penicillins"), the 'reaction.substance' element could be used to code the specific substance that was identified as having caused the reaction (for example, "amoxycillin"). Duplication of the value in the 'code' and 'reaction.substance' elements is acceptable when a specific substance has been recorded in 'code'.</t>
   </si>
   <si>
+    <t>example</t>
+  </si>
+  <si>
     <t>Codes defining the type of the substance (including pharmaceutical products).</t>
   </si>
   <si>
@@ -940,9 +943,6 @@
   </si>
   <si>
     <t>Manifestation can be expressed as a single word, phrase or brief description. For example: nausea, rash or no reaction. It is preferable that manifestation should be coded with a terminology, where possible. The values entered here may be used to display on an application screen as part of a list of adverse reactions, as recommended in the UK NHS CUI guidelines.  Terminologies commonly used include, but are not limited to, SNOMED CT or ICD10.</t>
-  </si>
-  <si>
-    <t>Clinical symptoms and/or signs that are observed or associated with an Adverse Reaction Event.</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/clinical-findings</t>
@@ -1159,6 +1159,21 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="22"/>
+        <i val="true"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -1500,7 +1515,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
         <v>30</v>
       </c>
@@ -1608,7 +1623,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
         <v>84</v>
       </c>
@@ -1716,7 +1731,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
         <v>92</v>
       </c>
@@ -1822,7 +1837,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
         <v>98</v>
       </c>
@@ -1930,7 +1945,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
         <v>104</v>
       </c>
@@ -2038,7 +2053,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
         <v>113</v>
       </c>
@@ -2146,7 +2161,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
         <v>121</v>
       </c>
@@ -2254,7 +2269,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
         <v>129</v>
       </c>
@@ -2362,7 +2377,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
         <v>137</v>
       </c>
@@ -2472,7 +2487,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
         <v>142</v>
       </c>
@@ -2598,7 +2613,7 @@
         <v>85</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>86</v>
@@ -2706,7 +2721,7 @@
         <v>85</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H13" t="s" s="2">
         <v>86</v>
@@ -2798,7 +2813,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
         <v>168</v>
       </c>
@@ -2922,7 +2937,7 @@
         <v>77</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>78</v>
@@ -3030,7 +3045,7 @@
         <v>85</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>78</v>
@@ -3132,13 +3147,13 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="F17" t="s" s="2">
         <v>85</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>78</v>
@@ -3184,11 +3199,9 @@
       <c r="W17" t="s" s="2">
         <v>202</v>
       </c>
-      <c r="X17" t="s" s="2">
+      <c r="X17" s="2"/>
+      <c r="Y17" t="s" s="2">
         <v>203</v>
-      </c>
-      <c r="Y17" t="s" s="2">
-        <v>204</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>78</v>
@@ -3221,22 +3234,22 @@
         <v>97</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="AK17" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="AK17" t="s" s="2">
+      <c r="AL17" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="AL17" t="s" s="2">
-        <v>207</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -3246,7 +3259,7 @@
         <v>85</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>78</v>
@@ -3255,13 +3268,13 @@
         <v>86</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="L18" t="s" s="2">
         <v>211</v>
-      </c>
-      <c r="L18" t="s" s="2">
-        <v>212</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3312,7 +3325,7 @@
         <v>78</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>85</v>
@@ -3327,18 +3340,18 @@
         <v>97</v>
       </c>
       <c r="AJ18" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="AK18" t="s" s="2">
         <v>213</v>
       </c>
-      <c r="AK18" t="s" s="2">
+      <c r="AL18" t="s" s="2">
         <v>214</v>
       </c>
-      <c r="AL18" t="s" s="2">
+    </row>
+    <row r="19" hidden="true">
+      <c r="A19" t="s" s="2">
         <v>215</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="2">
-        <v>216</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3361,13 +3374,13 @@
         <v>78</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="K19" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="L19" t="s" s="2">
         <v>218</v>
-      </c>
-      <c r="L19" t="s" s="2">
-        <v>219</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3418,7 +3431,7 @@
         <v>78</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>76</v>
@@ -3433,18 +3446,18 @@
         <v>97</v>
       </c>
       <c r="AJ19" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="AK19" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="AK19" t="s" s="2">
+      <c r="AL19" t="s" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" hidden="true">
+      <c r="A20" t="s" s="2">
         <v>221</v>
-      </c>
-      <c r="AL19" t="s" s="2">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="2">
-        <v>222</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3467,13 +3480,13 @@
         <v>78</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="L20" t="s" s="2">
         <v>224</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>225</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -3524,7 +3537,7 @@
         <v>78</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>76</v>
@@ -3539,18 +3552,18 @@
         <v>97</v>
       </c>
       <c r="AJ20" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="AK20" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="AK20" t="s" s="2">
+      <c r="AL20" t="s" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" hidden="true">
+      <c r="A21" t="s" s="2">
         <v>227</v>
-      </c>
-      <c r="AL20" t="s" s="2">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="2">
-        <v>228</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3573,13 +3586,13 @@
         <v>78</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="K21" t="s" s="2">
         <v>229</v>
       </c>
-      <c r="K21" t="s" s="2">
+      <c r="L21" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="L21" t="s" s="2">
-        <v>231</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3630,7 +3643,7 @@
         <v>78</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>76</v>
@@ -3645,22 +3658,22 @@
         <v>97</v>
       </c>
       <c r="AJ21" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="AK21" t="s" s="2">
         <v>232</v>
       </c>
-      <c r="AK21" t="s" s="2">
+      <c r="AL21" t="s" s="2">
         <v>233</v>
       </c>
-      <c r="AL21" t="s" s="2">
+    </row>
+    <row r="22" hidden="true">
+      <c r="A22" t="s" s="2">
         <v>234</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="2">
-        <v>235</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -3679,13 +3692,13 @@
         <v>78</v>
       </c>
       <c r="J22" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="K22" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="K22" t="s" s="2">
+      <c r="L22" t="s" s="2">
         <v>238</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>239</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3736,7 +3749,7 @@
         <v>78</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>76</v>
@@ -3751,22 +3764,22 @@
         <v>97</v>
       </c>
       <c r="AJ22" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AK22" t="s" s="2">
         <v>240</v>
       </c>
-      <c r="AK22" t="s" s="2">
+      <c r="AL22" t="s" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" hidden="true">
+      <c r="A23" t="s" s="2">
         <v>241</v>
-      </c>
-      <c r="AL22" t="s" s="2">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="2">
-        <v>242</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
@@ -3785,16 +3798,16 @@
         <v>86</v>
       </c>
       <c r="J23" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="K23" t="s" s="2">
         <v>244</v>
       </c>
-      <c r="K23" t="s" s="2">
+      <c r="L23" t="s" s="2">
         <v>245</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>246</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>247</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -3844,7 +3857,7 @@
         <v>78</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>76</v>
@@ -3859,18 +3872,18 @@
         <v>97</v>
       </c>
       <c r="AJ23" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="AK23" t="s" s="2">
         <v>248</v>
       </c>
-      <c r="AK23" t="s" s="2">
+      <c r="AL23" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="AL23" t="s" s="2">
+    </row>
+    <row r="24" hidden="true">
+      <c r="A24" t="s" s="2">
         <v>250</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="2">
-        <v>251</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3893,16 +3906,16 @@
         <v>78</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="L24" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="L24" t="s" s="2">
+      <c r="M24" t="s" s="2">
         <v>253</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>254</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -3952,7 +3965,7 @@
         <v>78</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>76</v>
@@ -3967,18 +3980,18 @@
         <v>97</v>
       </c>
       <c r="AJ24" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="AK24" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AL24" t="s" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" hidden="true">
+      <c r="A25" t="s" s="2">
         <v>255</v>
-      </c>
-      <c r="AK24" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AL24" t="s" s="2">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="2">
-        <v>256</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4001,16 +4014,16 @@
         <v>78</v>
       </c>
       <c r="J25" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="K25" t="s" s="2">
         <v>257</v>
       </c>
-      <c r="K25" t="s" s="2">
+      <c r="L25" t="s" s="2">
         <v>258</v>
       </c>
-      <c r="L25" t="s" s="2">
+      <c r="M25" t="s" s="2">
         <v>259</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
@@ -4060,7 +4073,7 @@
         <v>78</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>76</v>
@@ -4075,7 +4088,7 @@
         <v>97</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>78</v>
@@ -4086,7 +4099,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4100,7 +4113,7 @@
         <v>77</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>78</v>
@@ -4109,13 +4122,13 @@
         <v>78</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="K26" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="K26" t="s" s="2">
+      <c r="L26" t="s" s="2">
         <v>264</v>
-      </c>
-      <c r="L26" t="s" s="2">
-        <v>265</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -4166,7 +4179,7 @@
         <v>78</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>76</v>
@@ -4181,18 +4194,18 @@
         <v>97</v>
       </c>
       <c r="AJ26" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="AK26" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AL26" t="s" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" hidden="true">
+      <c r="A27" t="s" s="2">
         <v>266</v>
-      </c>
-      <c r="AK26" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AL26" t="s" s="2">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s" s="2">
-        <v>267</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4218,10 +4231,10 @@
         <v>87</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="L27" t="s" s="2">
         <v>268</v>
-      </c>
-      <c r="L27" t="s" s="2">
-        <v>269</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4272,7 +4285,7 @@
         <v>78</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>76</v>
@@ -4287,18 +4300,18 @@
         <v>78</v>
       </c>
       <c r="AJ27" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="AK27" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AL27" t="s" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" hidden="true">
+      <c r="A28" t="s" s="2">
         <v>271</v>
-      </c>
-      <c r="AK27" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AL27" t="s" s="2">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="2">
-        <v>272</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4327,7 +4340,7 @@
         <v>132</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M28" t="s" s="2">
         <v>134</v>
@@ -4380,7 +4393,7 @@
         <v>78</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>76</v>
@@ -4395,7 +4408,7 @@
         <v>136</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>78</v>
@@ -4404,13 +4417,13 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
@@ -4432,10 +4445,10 @@
         <v>131</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>277</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>278</v>
       </c>
       <c r="M29" t="s" s="2">
         <v>134</v>
@@ -4490,7 +4503,7 @@
         <v>78</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>76</v>
@@ -4514,9 +4527,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4542,13 +4555,13 @@
         <v>152</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L30" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>282</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>283</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -4574,7 +4587,7 @@
         <v>78</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>202</v>
+        <v>283</v>
       </c>
       <c r="X30" t="s" s="2">
         <v>284</v>
@@ -4598,7 +4611,7 @@
         <v>78</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>76</v>
@@ -4638,7 +4651,7 @@
         <v>77</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>78</v>
@@ -4684,11 +4697,9 @@
       <c r="W31" t="s" s="2">
         <v>202</v>
       </c>
-      <c r="X31" t="s" s="2">
+      <c r="X31" s="2"/>
+      <c r="Y31" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="Y31" t="s" s="2">
-        <v>293</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>78</v>
@@ -4727,16 +4738,16 @@
         <v>78</v>
       </c>
       <c r="AL31" t="s" s="2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="32" hidden="true">
+      <c r="A32" t="s" s="2">
         <v>294</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="2">
-        <v>295</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
@@ -4758,13 +4769,13 @@
         <v>87</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>297</v>
       </c>
-      <c r="L32" t="s" s="2">
+      <c r="M32" t="s" s="2">
         <v>298</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>299</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -4814,7 +4825,7 @@
         <v>78</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>76</v>
@@ -4829,18 +4840,18 @@
         <v>97</v>
       </c>
       <c r="AJ32" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="AK32" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AL32" t="s" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" hidden="true">
+      <c r="A33" t="s" s="2">
         <v>300</v>
-      </c>
-      <c r="AK32" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AL32" t="s" s="2">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s" s="2">
-        <v>301</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4863,13 +4874,13 @@
         <v>78</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -4920,7 +4931,7 @@
         <v>78</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>76</v>
@@ -4935,18 +4946,18 @@
         <v>97</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AL33" t="s" s="2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="34" hidden="true">
+      <c r="A34" t="s" s="2">
         <v>304</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s" s="2">
-        <v>305</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4972,13 +4983,13 @@
         <v>105</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>306</v>
       </c>
-      <c r="L34" t="s" s="2">
+      <c r="M34" t="s" s="2">
         <v>307</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>308</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
@@ -5007,11 +5018,11 @@
         <v>156</v>
       </c>
       <c r="X34" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="Y34" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="Y34" t="s" s="2">
-        <v>310</v>
-      </c>
       <c r="Z34" t="s" s="2">
         <v>78</v>
       </c>
@@ -5028,7 +5039,7 @@
         <v>78</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>76</v>
@@ -5052,9 +5063,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5080,13 +5091,13 @@
         <v>152</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>312</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>313</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>314</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
@@ -5112,14 +5123,14 @@
         <v>78</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>202</v>
+        <v>283</v>
       </c>
       <c r="X35" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="Y35" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="Y35" t="s" s="2">
-        <v>316</v>
-      </c>
       <c r="Z35" t="s" s="2">
         <v>78</v>
       </c>
@@ -5136,7 +5147,7 @@
         <v>78</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>76</v>
@@ -5151,18 +5162,18 @@
         <v>97</v>
       </c>
       <c r="AJ35" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="AK35" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AL35" t="s" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" hidden="true">
+      <c r="A36" t="s" s="2">
         <v>317</v>
-      </c>
-      <c r="AK35" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AL35" t="s" s="2">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s" s="2">
-        <v>318</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5185,16 +5196,16 @@
         <v>78</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>319</v>
       </c>
-      <c r="L36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>321</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
@@ -5244,7 +5255,7 @@
         <v>78</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>76</v>
@@ -5259,7 +5270,7 @@
         <v>97</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>78</v>
@@ -5269,6 +5280,24 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AL36">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="26">
+      <filters blank="true"/>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="A2:AI35">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$G2&lt;&gt;"Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$Q2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>